<commit_message>
ADX-764 Regenerate all necessary templates
</commit_message>
<xml_diff>
--- a/excel_templates/Country Estimates 2022/survey-template-v2.1.xlsx
+++ b/excel_templates/Country Estimates 2022/survey-template-v2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Column Definitions" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">UNAIDS Survey Indicators Input | Data Template</t>
   </si>
   <si>
-    <t xml:space="preserve">version 2.1; 2020-11-10</t>
+    <t xml:space="preserve">version 2.1; 2021-11-23</t>
   </si>
   <si>
     <t xml:space="preserve">Please use the following definitions to fill in the template overleaf. If data does not exist, please indicate so with the value "NA" and ignore any warning given by Excel.</t>
@@ -273,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,11 +290,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -377,14 +385,14 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="48.39"/>
@@ -421,7 +429,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -441,286 +449,286 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="D8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="D9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="D10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="D11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="E12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="D15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="D16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="D17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="E18" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="D19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="D20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="E21" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
@@ -756,73 +764,56 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.07"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="7" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>